<commit_message>
Report summary display and where clause application
</commit_message>
<xml_diff>
--- a/paperpusher/tests/Test report.xlsx
+++ b/paperpusher/tests/Test report.xlsx
@@ -7,15 +7,123 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Page one" sheetId="1" r:id="rId1"/>
+    <sheet name="Raw data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+  <si>
+    <t>Birth to last vote</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Objective</t>
+  </si>
+  <si>
+    <t>Objective met</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Minimum</t>
+  </si>
+  <si>
+    <t>Maximum</t>
+  </si>
+  <si>
+    <t>Less than 100</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>---</t>
+  </si>
+  <si>
+    <t>Birth to last vote for David</t>
+  </si>
+  <si>
+    <t>At least 150</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Last name begins with C</t>
+  </si>
+  <si>
+    <t>Last name</t>
+  </si>
+  <si>
+    <t>Date of birth</t>
+  </si>
+  <si>
+    <t>First name</t>
+  </si>
+  <si>
+    <t>Last date voted</t>
+  </si>
+  <si>
+    <t>Has first name</t>
+  </si>
+  <si>
+    <t>Is test?</t>
+  </si>
+  <si>
+    <t>Henderson</t>
+  </si>
+  <si>
+    <t>5/4/1982</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>11/10/2012</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>Cruz</t>
+  </si>
+  <si>
+    <t>9/27/1979</t>
+  </si>
+  <si>
+    <t>Leive</t>
+  </si>
+  <si>
+    <t>8/31/1977</t>
+  </si>
+  <si>
+    <t>Eric</t>
+  </si>
+  <si>
+    <t>9/25/2002</t>
+  </si>
+  <si>
+    <t>8/17/1947</t>
+  </si>
+  <si>
+    <t>Cora</t>
+  </si>
+  <si>
+    <t>6/20/2005</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -23,16 +131,71 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF008800"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEEEEE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFDDDD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDFFDD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -40,12 +203,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -340,12 +533,243 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3">
+        <v>13810.3333333333</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3">
+        <v>9156</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3">
+        <v>21127</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="B9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="3">
+        <v>11148</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B8:D8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2">
+        <v>11148</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4">
+        <v>9156</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5">
+        <v>21127</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added sum method for summary variables
</commit_message>
<xml_diff>
--- a/paperpusher/tests/Test report.xlsx
+++ b/paperpusher/tests/Test report.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\paperpusher\paperpusher\tests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
@@ -15,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
   <si>
     <t>Birth to last vote</t>
   </si>
@@ -47,6 +52,15 @@
     <t>---</t>
   </si>
   <si>
+    <t>Last name begins with C</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>At least 2</t>
+  </si>
+  <si>
     <t>Birth to last vote for David</t>
   </si>
   <si>
@@ -54,9 +68,6 @@
   </si>
   <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>Last name begins with C</t>
   </si>
   <si>
     <t>Last name</t>
@@ -122,8 +133,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,9 +235,6 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -239,12 +247,23 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -291,7 +310,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -323,9 +342,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -357,6 +377,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -532,149 +553,202 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="B2" s="2" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3">
-        <v>13810.3333333333</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="2">
+        <v>13810.333333333299</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>9156</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>21127</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="B8" s="1" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="B9" s="2" t="s">
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B15" s="2">
         <v>11148</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>12</v>
+      <c r="C15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B13:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11148</v>
       </c>
@@ -682,42 +756,42 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>9156</v>
       </c>
@@ -725,25 +799,25 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>21127</v>
       </c>
@@ -751,22 +825,22 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Percentage of total summary options
</commit_message>
<xml_diff>
--- a/paperpusher/tests/Test report.xlsx
+++ b/paperpusher/tests/Test report.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\paperpusher\paperpusher\tests\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
@@ -133,8 +128,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,6 +230,9 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -247,23 +245,12 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -310,7 +297,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -342,10 +329,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -377,7 +363,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -553,142 +538,134 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2">
-        <v>13810.333333333299</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="3">
+        <v>13810.3333333333</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:4">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="3">
         <v>9156</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:4">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="3">
         <v>21127</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
+    <row r="8" spans="1:4">
+      <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="B9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:4">
+      <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
+    <row r="13" spans="1:4">
+      <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="B14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:4">
+      <c r="A15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="3">
         <v>11148</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="5" t="s">
         <v>15</v>
       </c>
     </row>
@@ -703,26 +680,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -748,7 +713,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>11148</v>
       </c>
@@ -774,7 +739,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="B3">
         <v>1</v>
       </c>
@@ -791,7 +756,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>9156</v>
       </c>
@@ -817,7 +782,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>21127</v>
       </c>

</xml_diff>

<commit_message>
Fixed issue where SummarySection.summary_variable included variables for all sections
</commit_message>
<xml_diff>
--- a/paperpusher/tests/Test report.xlsx
+++ b/paperpusher/tests/Test report.xlsx
@@ -17,21 +17,42 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
   <si>
+    <t>Last name begins with C</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Objective</t>
+  </si>
+  <si>
+    <t>Objective met</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>At least 2</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Birth to last vote for David</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>At least 150</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>Birth to last vote</t>
   </si>
   <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Objective</t>
-  </si>
-  <si>
-    <t>Objective met</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
     <t>Minimum</t>
   </si>
   <si>
@@ -41,28 +62,7 @@
     <t>Less than 100</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>---</t>
-  </si>
-  <si>
-    <t>Last name begins with C</t>
-  </si>
-  <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>At least 2</t>
-  </si>
-  <si>
-    <t>Birth to last vote for David</t>
-  </si>
-  <si>
-    <t>At least 150</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>Last name</t>
@@ -568,112 +568,112 @@
         <v>4</v>
       </c>
       <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="B7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="3">
+        <v>11148</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="B12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="3">
         <v>13810.3333333333</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3">
+      <c r="C13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3">
         <v>9156</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="3">
-        <v>21127</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="B8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="B9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="3">
-        <v>1</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="B13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="B14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>3</v>
+      <c r="C14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B15" s="3">
-        <v>11148</v>
+        <v>21127</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -689,10 +689,10 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
       </c>
       <c r="C1" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Report summary variables by group
</commit_message>
<xml_diff>
--- a/paperpusher/tests/Test report.xlsx
+++ b/paperpusher/tests/Test report.xlsx
@@ -15,54 +15,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
+  <si>
+    <t>Objectives</t>
+  </si>
+  <si>
+    <t>Objective</t>
+  </si>
+  <si>
+    <t>Met</t>
+  </si>
+  <si>
+    <t>Birth to last vote average less than 100</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>More 2 or more people with last name beginning with C</t>
+  </si>
+  <si>
+    <t>Birth to last vote</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Minimum</t>
+  </si>
+  <si>
+    <t>Maximum</t>
+  </si>
+  <si>
+    <t>All observations</t>
+  </si>
   <si>
     <t>Last name begins with C</t>
   </si>
   <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Objective</t>
-  </si>
-  <si>
-    <t>Objective met</t>
-  </si>
-  <si>
     <t>Sum</t>
   </si>
   <si>
-    <t>At least 2</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Birth to last vote for David</t>
   </si>
   <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>At least 150</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Birth to last vote</t>
-  </si>
-  <si>
-    <t>Minimum</t>
-  </si>
-  <si>
-    <t>Maximum</t>
-  </si>
-  <si>
-    <t>Less than 100</t>
-  </si>
-  <si>
-    <t>---</t>
+    <t>First name David</t>
   </si>
   <si>
     <t>Last name</t>
@@ -129,7 +129,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,16 +160,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF008800"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,12 +183,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFDDDD"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDFFDD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -228,7 +214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -240,9 +226,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -539,141 +522,128 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="B4" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="3">
+        <v>13810.3333333333</v>
+      </c>
+      <c r="C8" s="3">
+        <v>9156</v>
+      </c>
+      <c r="D8" s="3">
+        <v>21127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3">
         <v>1</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="2" t="s">
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="3">
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="3">
         <v>11148</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="B11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="B12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="3">
-        <v>13810.3333333333</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="3">
-        <v>9156</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="3">
-        <v>21127</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>15</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B11:D11"/>
+  <mergeCells count="4">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A16:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -689,10 +659,10 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Support for bar charts
</commit_message>
<xml_diff>
--- a/paperpusher/tests/Test report.xlsx
+++ b/paperpusher/tests/Test report.xlsx
@@ -217,16 +217,16 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -527,6 +527,11 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="6" width="30.7109375" customWidth="1"/>
+    <col min="1" max="11" width="30.7109375" customWidth="1"/>
+    <col min="1" max="16" width="30.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
Added properties to the report builder controller
</commit_message>
<xml_diff>
--- a/paperpusher/tests/Test report.xlsx
+++ b/paperpusher/tests/Test report.xlsx
@@ -26,13 +26,13 @@
     <t>Met</t>
   </si>
   <si>
+    <t>More 2 or more people with last name beginning with C</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
     <t>Birth to last vote average less than 100</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>More 2 or more people with last name beginning with C</t>
   </si>
   <si>
     <t>Birth to last vote for David</t>

</xml_diff>